<commit_message>
UPDATE BUDGET TO FIT RANGE
</commit_message>
<xml_diff>
--- a/CleanedData/SalesBudget.xlsx
+++ b/CleanedData/SalesBudget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\720350\Desktop\Data Analyst Portfolio Data\Sales\3 - Cleansing &amp; Transformation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0fed3bb5cd6e0636/Documents/Pessoal/Estudos/DataAnalisys/SalesAnalysisProject_LocalRepository/CleanedData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB0F426-EAE3-4CAE-A364-B68B0189A02A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{9DB0F426-EAE3-4CAE-A364-B68B0189A02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6101FE09-FEC5-4B80-BD6D-D60BEBB47BDB}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="1995" windowWidth="15900" windowHeight="14805" xr2:uid="{5CABF058-C44E-4B4C-A322-6CA47C838A4D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5CABF058-C44E-4B4C-A322-6CA47C838A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Budget" sheetId="1" r:id="rId1"/>
@@ -45,8 +45,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -99,11 +100,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -419,19 +421,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D3E0CB-37F1-4778-A2AE-5F0FF4562B38}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>43831</v>
       </c>
@@ -447,7 +449,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>43862</v>
       </c>
@@ -455,7 +457,7 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>43891</v>
       </c>
@@ -463,7 +465,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>43922</v>
       </c>
@@ -471,7 +473,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>43952</v>
       </c>
@@ -479,7 +481,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>43983</v>
       </c>
@@ -487,7 +489,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44013</v>
       </c>
@@ -495,7 +497,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>44044</v>
       </c>
@@ -503,7 +505,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>44075</v>
       </c>
@@ -511,7 +513,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>44105</v>
       </c>
@@ -519,7 +521,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>44136</v>
       </c>
@@ -527,7 +529,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>44166</v>
       </c>
@@ -535,52 +537,293 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>44197</v>
       </c>
       <c r="B14" s="2">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>840000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44228</v>
       </c>
       <c r="B15" s="2">
-        <v>800000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>840000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>44256</v>
       </c>
       <c r="B16" s="2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>44287</v>
       </c>
       <c r="B17" s="2">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>44317</v>
       </c>
       <c r="B18" s="2">
-        <v>1100000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1155000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>44348</v>
       </c>
       <c r="B19" s="2">
-        <v>1100000</v>
+        <v>1155000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>44378</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>44409</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>44440</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>44470</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>44501</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1575000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>44531</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2100000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>44562</v>
+      </c>
+      <c r="B26" s="2">
+        <v>882000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>44593</v>
+      </c>
+      <c r="B27" s="2">
+        <v>882000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>44621</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1102500</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>44652</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1102500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>44682</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1212750</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>44713</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1212750</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>44743</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1653750</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>44774</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1653750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>44805</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1653750</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
+        <v>44835</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1653750</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>44866</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1653750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
+        <v>44896</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2205000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>44927</v>
+      </c>
+      <c r="B38" s="4">
+        <f>1.025*B26</f>
+        <v>904049.99999999988</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>44958</v>
+      </c>
+      <c r="B39" s="4">
+        <v>904049.99999999988</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>44986</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1130062.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
+        <v>45017</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1130062.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>45047</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1243068.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
+        <v>45078</v>
+      </c>
+      <c r="B43" s="4">
+        <v>1243068.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>45108</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1695093.7499999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="3">
+        <v>45139</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1695093.7499999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>45170</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1695093.7499999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="3">
+        <v>45200</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1695093.7499999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>45231</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1695093.7499999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>45261</v>
+      </c>
+      <c r="B49" s="4">
+        <v>2260125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>